<commit_message>
delete p3 due to IMU recording only for second ascent
</commit_message>
<xml_diff>
--- a/demographic_data.xlsx
+++ b/demographic_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dorot\Desktop\MasterStudy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB00B13C-A586-493E-A878-52D5281F49BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6525FE2-46F6-4DA4-B0C3-3C1634C78B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="15">
   <si>
     <t>IDN</t>
   </si>
@@ -387,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -485,22 +485,22 @@
         <v>14</v>
       </c>
       <c r="C4">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D4">
-        <v>157</v>
+        <v>168</v>
       </c>
       <c r="E4">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G4">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -508,22 +508,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G5">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H5">
         <v>1.5</v>
@@ -534,25 +534,25 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D6">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E6">
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G6">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H6">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -563,22 +563,22 @@
         <v>14</v>
       </c>
       <c r="C7">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="E7">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G7">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="H7">
-        <v>2.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -589,22 +589,22 @@
         <v>14</v>
       </c>
       <c r="C8">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D8">
         <v>170</v>
       </c>
       <c r="E8">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G8">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H8">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -612,25 +612,25 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9">
         <v>25</v>
       </c>
       <c r="D9">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="E9">
+        <v>19</v>
+      </c>
+      <c r="F9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9">
         <v>16</v>
       </c>
-      <c r="F9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G9">
-        <v>13</v>
-      </c>
       <c r="H9">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -644,10 +644,10 @@
         <v>25</v>
       </c>
       <c r="D10">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E10">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="F10" t="s">
         <v>9</v>
@@ -656,7 +656,7 @@
         <v>16</v>
       </c>
       <c r="H10">
-        <v>3</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -667,13 +667,13 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D11">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="E11">
-        <v>6</v>
+        <v>1.5</v>
       </c>
       <c r="F11" t="s">
         <v>9</v>
@@ -682,7 +682,7 @@
         <v>16</v>
       </c>
       <c r="H11">
-        <v>2.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -693,22 +693,22 @@
         <v>13</v>
       </c>
       <c r="C12">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D12">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="E12">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12">
+        <v>15</v>
+      </c>
+      <c r="H12">
         <v>1.5</v>
-      </c>
-      <c r="F12" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12">
-        <v>16</v>
-      </c>
-      <c r="H12">
-        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -716,25 +716,25 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C13">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D13">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="F13" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G13">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H13">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -745,22 +745,22 @@
         <v>14</v>
       </c>
       <c r="C14">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D14">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="E14">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G14">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -771,22 +771,22 @@
         <v>14</v>
       </c>
       <c r="C15">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D15">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E15">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G15">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H15">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -794,16 +794,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="D16">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="E16">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F16" t="s">
         <v>5</v>
@@ -812,7 +812,7 @@
         <v>13</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -823,47 +823,21 @@
         <v>13</v>
       </c>
       <c r="C17">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D17">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="E17">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="F17" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G17">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H17">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>13</v>
-      </c>
-      <c r="C18">
-        <v>34</v>
-      </c>
-      <c r="D18">
-        <v>169</v>
-      </c>
-      <c r="E18">
-        <v>17</v>
-      </c>
-      <c r="F18" t="s">
-        <v>7</v>
-      </c>
-      <c r="G18">
-        <v>17</v>
-      </c>
-      <c r="H18">
         <v>1.5</v>
       </c>
     </row>

</xml_diff>